<commit_message>
feat: Add example resource query script and enhance data service functionality
- Introduced `example_resource_query.py` to demonstrate usage of `find_best_resource()` from `DataService`.
- Updated `test_receipt.py` to improve receipt printing logic and removed unused `ReceiptData`.
- Created `test_resource_query.py` for testing resource query functionality with various weight configurations.
- Enhanced `DataService` to load resources from Excel and calculate prevalent mindsets.
- Refactored `figurine_service.py` to utilize new receipt generation logic and removed dependency on `receipt_template.py`.
- Deleted `receipt_template.py` as its functionality has been integrated into `slip_printing.py`.
- Updated `slip_printing.py` to include new methods for printing images and labeled sections.
</commit_message>
<xml_diff>
--- a/assets/Unfinished_data_collection.xlsx
+++ b/assets/Unfinished_data_collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mindsets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="426">
   <si>
     <t xml:space="preserve">Mindset_ID</t>
   </si>
@@ -533,13 +533,10 @@
     <t xml:space="preserve">Link</t>
   </si>
   <si>
-    <t xml:space="preserve">Mindsets (M01–M04)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedürfnisse (A23–A28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aktuelle Situation (A29–A33)</t>
+    <t xml:space="preserve">Bedürfnisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Situation</t>
   </si>
   <si>
     <t xml:space="preserve">Tools &amp; Inspiration</t>
@@ -1405,6 +1402,7 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1473,7 +1471,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1759,6 +1757,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.07"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1855,13 +1856,14 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="65.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="70.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="37.99"/>
@@ -1916,7 +1918,7 @@
       <c r="G2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2039,7 +2041,7 @@
       <c r="G8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2145,7 +2147,7 @@
       <c r="G13" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2368,7 +2370,7 @@
       <c r="G24" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="5" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2488,7 +2490,7 @@
       <c r="G30" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="5" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2578,11 +2580,18 @@
   </sheetPr>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="38.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="68.44"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2595,350 +2604,350 @@
         <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>161</v>
@@ -2946,495 +2955,495 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>148</v>
@@ -3442,16 +3451,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>152</v>
@@ -3459,33 +3468,33 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>155</v>
@@ -3493,16 +3502,16 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>161</v>
@@ -3510,138 +3519,138 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="F56" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3670,37 +3679,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="1612.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="1358.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="1209.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="434.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="926.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3735,818 +3744,818 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enhance content generation and shape rendering with new features and tests
</commit_message>
<xml_diff>
--- a/assets/Unfinished_data_collection.xlsx
+++ b/assets/Unfinished_data_collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mindsets" sheetId="1" state="visible" r:id="rId3"/>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Explorer, Sensemaker</t>
   </si>
   <si>
-    <t xml:space="preserve">circle</t>
+    <t xml:space="preserve">semioval</t>
   </si>
   <si>
     <t xml:space="preserve">A02</t>
@@ -248,6 +248,9 @@
     <t xml:space="preserve">Explorer, Strategist</t>
   </si>
   <si>
+    <t xml:space="preserve">sphere_circle</t>
+  </si>
+  <si>
     <t xml:space="preserve">A08</t>
   </si>
   <si>
@@ -302,7 +305,7 @@
     <t xml:space="preserve">Experiencer</t>
   </si>
   <si>
-    <t xml:space="preserve">trapezoid_wide</t>
+    <t xml:space="preserve">wide_rectangle</t>
   </si>
   <si>
     <t xml:space="preserve">A13</t>
@@ -356,7 +359,7 @@
     <t xml:space="preserve">Die Person weicht Unsicherheiten tendenziell aus oder vermeidet sie.</t>
   </si>
   <si>
-    <t xml:space="preserve">diamond</t>
+    <t xml:space="preserve">stepped_block</t>
   </si>
   <si>
     <t xml:space="preserve">A18</t>
@@ -422,7 +425,7 @@
     <t xml:space="preserve">Experiencer, Explorer, Strategist, Sensemaker</t>
   </si>
   <si>
-    <t xml:space="preserve">triangle_down</t>
+    <t xml:space="preserve">solid_diamond</t>
   </si>
   <si>
     <t xml:space="preserve">A24</t>
@@ -483,9 +486,6 @@
   </si>
   <si>
     <t xml:space="preserve">Junge Menschen am Anfang ihres Berufslebens. Sie müssen ihre Position in der Arbeitswelt finden und wollen Erfahrung sammeln. Ihre Herausforderung ist es, einen Beruf oder Job zu finden, der zu ihren Stärken, ihrer Haltung und ihren Interessen passt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectangle_wide</t>
   </si>
   <si>
     <t xml:space="preserve">A30</t>
@@ -1402,7 +1402,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1758,7 +1757,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="45.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,14 +1855,14 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="65.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="58.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="70.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="37.99"/>
@@ -2042,24 +2041,24 @@
         <v>2</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>2</v>
@@ -2067,16 +2066,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>55</v>
@@ -2087,19 +2086,19 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>2</v>
@@ -2107,16 +2106,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>51</v>
@@ -2127,45 +2126,45 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>3</v>
@@ -2173,16 +2172,16 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>51</v>
@@ -2193,19 +2192,19 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>3</v>
@@ -2213,7 +2212,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>24</v>
@@ -2222,7 +2221,7 @@
         <v>64</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>3</v>
@@ -2230,39 +2229,39 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>4</v>
@@ -2270,16 +2269,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>59</v>
@@ -2290,16 +2289,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>55</v>
@@ -2310,19 +2309,19 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>4</v>
@@ -2330,16 +2329,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>55</v>
@@ -2350,45 +2349,45 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>5</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>5</v>
@@ -2396,19 +2395,19 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>5</v>
@@ -2416,19 +2415,19 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>5</v>
@@ -2436,19 +2435,19 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>5</v>
@@ -2456,16 +2455,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>5</v>
@@ -2473,25 +2472,25 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>6</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,17 +2579,17 @@
   </sheetPr>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="38.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="68.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="39.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="34.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="56.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="4" width="38.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="68.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,7 +2723,7 @@
         <v>191</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>171</v>
@@ -2764,7 +2763,7 @@
         <v>199</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>200</v>
@@ -2784,7 +2783,7 @@
         <v>202</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>203</v>
@@ -2844,7 +2843,7 @@
         <v>212</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>213</v>
@@ -3144,7 +3143,7 @@
         <v>263</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>264</v>
@@ -3164,7 +3163,7 @@
         <v>266</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>264</v>
@@ -3440,13 +3439,13 @@
         <v>296</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>231</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3457,7 +3456,7 @@
         <v>297</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>231</v>
@@ -3474,7 +3473,7 @@
         <v>298</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>231</v>
@@ -3491,7 +3490,7 @@
         <v>299</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>231</v>
@@ -3508,7 +3507,7 @@
         <v>300</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>231</v>
@@ -3671,43 +3670,46 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.3"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="1612.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="195.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="1358.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="165.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="1209.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="121.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="539.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="434.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="61.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="926.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="165.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>317</v>
       </c>
@@ -3730,8 +3732,8 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D112" activeCellId="0" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: Update Unfinished_data_collection.xlsx with new data for enhanced analysis
</commit_message>
<xml_diff>
--- a/assets/Unfinished_data_collection.xlsx
+++ b/assets/Unfinished_data_collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mindsets" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="431">
   <si>
     <t xml:space="preserve">Mindset_ID</t>
   </si>
@@ -191,6 +191,9 @@
     <t xml:space="preserve">Strategist</t>
   </si>
   <si>
+    <t xml:space="preserve">sphere_circle</t>
+  </si>
+  <si>
     <t xml:space="preserve">A03</t>
   </si>
   <si>
@@ -246,9 +249,6 @@
   </si>
   <si>
     <t xml:space="preserve">Explorer, Strategist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sphere_circle</t>
   </si>
   <si>
     <t xml:space="preserve">A08</t>
@@ -1462,25 +1462,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1682,7 +1674,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H31:H34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1698,47 +1690,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="2150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="2955.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="2851.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="2388.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1761,7 +1753,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H31:H34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1778,68 +1770,68 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1861,13 +1853,13 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="46.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,684 +1889,765 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="D5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="H5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="G10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="G20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="G27" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G24" s="0" t="n">
+      <c r="D28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="H28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="0" t="n">
+      <c r="D29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="2" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <v>5</v>
+      <c r="H29" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="H30" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="H33" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2596,7 +2669,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H31:H34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2622,1042 +2695,1042 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="2" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="2" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="2" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="2" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="D23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="2" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="2" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="2" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="2" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="D35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="2" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="F43" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" s="2" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="F49" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F52" s="0" t="s">
+      <c r="F52" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F53" s="0" t="s">
+      <c r="F53" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="F54" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" s="2" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3679,47 +3752,47 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H31:H34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="81.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="81.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="165.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="538.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="165.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>322</v>
       </c>
     </row>
@@ -3742,7 +3815,7 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H31:H34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3756,810 +3829,810 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="2" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="2" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="2" t="s">
         <v>410</v>
       </c>
     </row>

</xml_diff>